<commit_message>
visuals and author stuff
</commit_message>
<xml_diff>
--- a/originaldata/scratch.xlsx
+++ b/originaldata/scratch.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11540" yWindow="0" windowWidth="14060" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="4100" yWindow="0" windowWidth="21500" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="753">
   <si>
     <t>babiarzc.bib</t>
   </si>
@@ -936,15 +936,6 @@
     <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/bowserc.bib", </t>
   </si>
   <si>
-    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/boyle.bib", </t>
-  </si>
-  <si>
-    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/bradbury.bib", </t>
-  </si>
-  <si>
-    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/brasino.bib", </t>
-  </si>
-  <si>
     <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/bravoh.bib", </t>
   </si>
   <si>
@@ -954,21 +945,12 @@
     <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/cardiffm.bib", </t>
   </si>
   <si>
-    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/cherkauer.bib", </t>
-  </si>
-  <si>
     <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/clancyk.bib", </t>
   </si>
   <si>
     <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/clarya.bib", </t>
   </si>
   <si>
-    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/converse.bib", </t>
-  </si>
-  <si>
-    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/cruciani.bib", </t>
-  </si>
-  <si>
     <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/diebelm.bib", </t>
   </si>
   <si>
@@ -1011,9 +993,6 @@
     <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/hemmingj.bib", </t>
   </si>
   <si>
-    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/hoopes.bib", </t>
-  </si>
-  <si>
     <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/hooyert.bib", </t>
   </si>
   <si>
@@ -1035,9 +1014,6 @@
     <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/knobelochl.bib", </t>
   </si>
   <si>
-    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/kraft.bib", </t>
-  </si>
-  <si>
     <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/kucharikc.bib", </t>
   </si>
   <si>
@@ -1101,9 +1077,6 @@
     <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/mcmahonk.bib", </t>
   </si>
   <si>
-    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/muldoon.bib", </t>
-  </si>
-  <si>
     <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/nitkaa.bib", </t>
   </si>
   <si>
@@ -1128,12 +1101,6 @@
     <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/pedersenj.bib", </t>
   </si>
   <si>
-    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/peterson.bib", </t>
-  </si>
-  <si>
-    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/postle.bib", </t>
-  </si>
-  <si>
     <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/rabinowitzh.bib", </t>
   </si>
   <si>
@@ -1164,9 +1131,6 @@
     <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/skalbeckj.bib", </t>
   </si>
   <si>
-    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/sonzogni.bib", </t>
-  </si>
-  <si>
     <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/sorsak.bib", </t>
   </si>
   <si>
@@ -1179,21 +1143,12 @@
     <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/stoorr.bib", </t>
   </si>
   <si>
-    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/sucht.bib", </t>
-  </si>
-  <si>
     <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/swansons.bib", </t>
   </si>
   <si>
     <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/tangc.bib", </t>
   </si>
   <si>
-    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/trussell.bib", </t>
-  </si>
-  <si>
-    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/tyler.bib", </t>
-  </si>
-  <si>
     <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/underwoodc.bib", </t>
   </si>
   <si>
@@ -1210,6 +1165,1119 @@
   </si>
   <si>
     <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/zwolinskim.bib", </t>
+  </si>
+  <si>
+    <t>adamst.bib</t>
+  </si>
+  <si>
+    <t>albertsonp.bib</t>
+  </si>
+  <si>
+    <t>alhajjarb.bib</t>
+  </si>
+  <si>
+    <t>amesonp.bib</t>
+  </si>
+  <si>
+    <t>andersonm.bib</t>
+  </si>
+  <si>
+    <t>anklamj.bib</t>
+  </si>
+  <si>
+    <t>armstrongd.bib</t>
+  </si>
+  <si>
+    <t>attigj.bib</t>
+  </si>
+  <si>
+    <t>ayres.bib</t>
+  </si>
+  <si>
+    <t>baileyf.bib</t>
+  </si>
+  <si>
+    <t>battistaj.bib</t>
+  </si>
+  <si>
+    <t>Beaumiers.bib</t>
+  </si>
+  <si>
+    <t>beckerg.bib</t>
+  </si>
+  <si>
+    <t>belluckd.bib</t>
+  </si>
+  <si>
+    <t>bentleyc.bib</t>
+  </si>
+  <si>
+    <t>berndtj.bib</t>
+  </si>
+  <si>
+    <t>berthouexp.bib</t>
+  </si>
+  <si>
+    <t>blanchardm.bib</t>
+  </si>
+  <si>
+    <t>blondeg.bib</t>
+  </si>
+  <si>
+    <t>bohlingg.bib</t>
+  </si>
+  <si>
+    <t>bohnm.bib</t>
+  </si>
+  <si>
+    <t>bosscherp.bib</t>
+  </si>
+  <si>
+    <t>bowenb.bib</t>
+  </si>
+  <si>
+    <t>boyle copy.bib</t>
+  </si>
+  <si>
+    <t>bradbury copy.bib</t>
+  </si>
+  <si>
+    <t>bradburyk_prelim.bib</t>
+  </si>
+  <si>
+    <t>brasino copy.bib</t>
+  </si>
+  <si>
+    <t>breyk.bib</t>
+  </si>
+  <si>
+    <t>brownb.bib</t>
+  </si>
+  <si>
+    <t>browneb.bib</t>
+  </si>
+  <si>
+    <t>bubenzerg.bib</t>
+  </si>
+  <si>
+    <t>bundyl.bib</t>
+  </si>
+  <si>
+    <t>catesk.bib</t>
+  </si>
+  <si>
+    <t>chambersl.bib</t>
+  </si>
+  <si>
+    <t>changm.bib</t>
+  </si>
+  <si>
+    <t>chenc.bib</t>
+  </si>
+  <si>
+    <t>cherkauer copy.bib</t>
+  </si>
+  <si>
+    <t>chestersg.bib</t>
+  </si>
+  <si>
+    <t>collinsm.bib</t>
+  </si>
+  <si>
+    <t>connersk.bib</t>
+  </si>
+  <si>
+    <t>converse copy.bib</t>
+  </si>
+  <si>
+    <t>cowells.bib</t>
+  </si>
+  <si>
+    <t>cruciani copy.bib</t>
+  </si>
+  <si>
+    <t>curwend.bib</t>
+  </si>
+  <si>
+    <t>danielt.bib</t>
+  </si>
+  <si>
+    <t>davenportd.bib</t>
+  </si>
+  <si>
+    <t>davidsond.bib</t>
+  </si>
+  <si>
+    <t>delucad.bib</t>
+  </si>
+  <si>
+    <t>detroitd.bib</t>
+  </si>
+  <si>
+    <t>dobbinsb.bib</t>
+  </si>
+  <si>
+    <t>doranf.bib</t>
+  </si>
+  <si>
+    <t>doyled.bib</t>
+  </si>
+  <si>
+    <t>dunnj.bib</t>
+  </si>
+  <si>
+    <t>eatont.bib</t>
+  </si>
+  <si>
+    <t>eldanm.bib</t>
+  </si>
+  <si>
+    <t>evansw.bib</t>
+  </si>
+  <si>
+    <t>eykholtg.bib</t>
+  </si>
+  <si>
+    <t>falkp.bib</t>
+  </si>
+  <si>
+    <t>fathullar.bib</t>
+  </si>
+  <si>
+    <t>faublep.bib</t>
+  </si>
+  <si>
+    <t>feinsteind.bib</t>
+  </si>
+  <si>
+    <t>fermanichk.bib</t>
+  </si>
+  <si>
+    <t>fishers.bib</t>
+  </si>
+  <si>
+    <t>fitzgeraldc.bib</t>
+  </si>
+  <si>
+    <t>friedmanm.bib</t>
+  </si>
+  <si>
+    <t>fripiatj.bib</t>
+  </si>
+  <si>
+    <t>geiss.bib</t>
+  </si>
+  <si>
+    <t>gilbertt.bib</t>
+  </si>
+  <si>
+    <t>goodmani.bib</t>
+  </si>
+  <si>
+    <t>greent.bib</t>
+  </si>
+  <si>
+    <t>greerb.bib</t>
+  </si>
+  <si>
+    <t>grundlt.bib</t>
+  </si>
+  <si>
+    <t>hamr.bib</t>
+  </si>
+  <si>
+    <t>hansond.bib</t>
+  </si>
+  <si>
+    <t>harkinj.bib</t>
+  </si>
+  <si>
+    <t>harrism.bib</t>
+  </si>
+  <si>
+    <t>harrisr.bib</t>
+  </si>
+  <si>
+    <t>hartleyh.bib</t>
+  </si>
+  <si>
+    <t>hartleyj.bib</t>
+  </si>
+  <si>
+    <t>harveyr.bib</t>
+  </si>
+  <si>
+    <t>heitmanm.bib</t>
+  </si>
+  <si>
+    <t>helmkep.bib</t>
+  </si>
+  <si>
+    <t>holmand.bib</t>
+  </si>
+  <si>
+    <t>hoopes copy.bib</t>
+  </si>
+  <si>
+    <t>hungerc.bib</t>
+  </si>
+  <si>
+    <t>hutchinsonk.bib</t>
+  </si>
+  <si>
+    <t>jelinskid.bib</t>
+  </si>
+  <si>
+    <t>kammeld.bib</t>
+  </si>
+  <si>
+    <t>kammererp.bib</t>
+  </si>
+  <si>
+    <t>kanarekm.bib</t>
+  </si>
+  <si>
+    <t>karasovw.bib</t>
+  </si>
+  <si>
+    <t>kendye.bib</t>
+  </si>
+  <si>
+    <t>kentera.bib</t>
+  </si>
+  <si>
+    <t>knaakm.bib</t>
+  </si>
+  <si>
+    <t>kopecky.bib</t>
+  </si>
+  <si>
+    <t>kraft copy.bib</t>
+  </si>
+  <si>
+    <t>kraftg.bib</t>
+  </si>
+  <si>
+    <t>krohnc.bib</t>
+  </si>
+  <si>
+    <t>kruele.bib</t>
+  </si>
+  <si>
+    <t>lanl.bib</t>
+  </si>
+  <si>
+    <t>lantzw.bib</t>
+  </si>
+  <si>
+    <t>lawrencej.bib</t>
+  </si>
+  <si>
+    <t>lemastersg.bib</t>
+  </si>
+  <si>
+    <t>levyj.bib</t>
+  </si>
+  <si>
+    <t>mccallisterr.bib</t>
+  </si>
+  <si>
+    <t>mcgrathr.bib</t>
+  </si>
+  <si>
+    <t>mckereghanp.bib</t>
+  </si>
+  <si>
+    <t>mckinleyw.bib</t>
+  </si>
+  <si>
+    <t>mechenichd.bib</t>
+  </si>
+  <si>
+    <t>meisnerl.bib</t>
+  </si>
+  <si>
+    <t>melbyj.bib</t>
+  </si>
+  <si>
+    <t>mickelsond.bib</t>
+  </si>
+  <si>
+    <t>monkmeyerp.bib</t>
+  </si>
+  <si>
+    <t>mudreym.bib</t>
+  </si>
+  <si>
+    <t>muhannaa.bib</t>
+  </si>
+  <si>
+    <t>muldoon copy.bib</t>
+  </si>
+  <si>
+    <t>murskyg.bib</t>
+  </si>
+  <si>
+    <t>newenhousea.bib</t>
+  </si>
+  <si>
+    <t>nienkeg.bib</t>
+  </si>
+  <si>
+    <t>niewoehnerj.bib</t>
+  </si>
+  <si>
+    <t>noelm.bib</t>
+  </si>
+  <si>
+    <t>nollr.bib</t>
+  </si>
+  <si>
+    <t>norenbergc.bib</t>
+  </si>
+  <si>
+    <t>nowakp.bib</t>
+  </si>
+  <si>
+    <t>omanb.bib</t>
+  </si>
+  <si>
+    <t>osbornet.bib</t>
+  </si>
+  <si>
+    <t>ostergrenc.bib</t>
+  </si>
+  <si>
+    <t>otisr.bib</t>
+  </si>
+  <si>
+    <t>palmerc.bib</t>
+  </si>
+  <si>
+    <t>parkj.bib</t>
+  </si>
+  <si>
+    <t>parsonsl.bib</t>
+  </si>
+  <si>
+    <t>patochj.bib</t>
+  </si>
+  <si>
+    <t>pauld.bib</t>
+  </si>
+  <si>
+    <t>pawloskia.bib</t>
+  </si>
+  <si>
+    <t>peerenboomd.bib</t>
+  </si>
+  <si>
+    <t>pelczarj.bib</t>
+  </si>
+  <si>
+    <t>peterson copy.bib</t>
+  </si>
+  <si>
+    <t>porterw.bib</t>
+  </si>
+  <si>
+    <t>portlet.bib</t>
+  </si>
+  <si>
+    <t>posnerj.bib</t>
+  </si>
+  <si>
+    <t>postle copy.bib</t>
+  </si>
+  <si>
+    <t>postlej.bib</t>
+  </si>
+  <si>
+    <t>potterk.bib</t>
+  </si>
+  <si>
+    <t>pughl.bib</t>
+  </si>
+  <si>
+    <t>readh.bib</t>
+  </si>
+  <si>
+    <t>richardsonn.bib</t>
+  </si>
+  <si>
+    <t>roloffb.bib</t>
+  </si>
+  <si>
+    <t>saltesj.bib</t>
+  </si>
+  <si>
+    <t>sandstroml.bib</t>
+  </si>
+  <si>
+    <t>sauerd.bib</t>
+  </si>
+  <si>
+    <t>schalchl.bib</t>
+  </si>
+  <si>
+    <t>schwalbej.bib</t>
+  </si>
+  <si>
+    <t>seyboldc.bib</t>
+  </si>
+  <si>
+    <t>shrawder.bib</t>
+  </si>
+  <si>
+    <t>simot.bib</t>
+  </si>
+  <si>
+    <t>simsimang.bib</t>
+  </si>
+  <si>
+    <t>singhp.bib</t>
+  </si>
+  <si>
+    <t>slanek.bib</t>
+  </si>
+  <si>
+    <t>smallg.bib</t>
+  </si>
+  <si>
+    <t>sonzogni copy.bib</t>
+  </si>
+  <si>
+    <t>sorensonj.bib</t>
+  </si>
+  <si>
+    <t>stieglitzr.bib</t>
+  </si>
+  <si>
+    <t>stollr.bib</t>
+  </si>
+  <si>
+    <t>strandridgej.bib</t>
+  </si>
+  <si>
+    <t>sucht copy.bib</t>
+  </si>
+  <si>
+    <t>suchtm.bib</t>
+  </si>
+  <si>
+    <t>svavarssong.bib</t>
+  </si>
+  <si>
+    <t>taylorr.bib</t>
+  </si>
+  <si>
+    <t>tinkerj.bib</t>
+  </si>
+  <si>
+    <t>trappp.bib</t>
+  </si>
+  <si>
+    <t>travism.bib</t>
+  </si>
+  <si>
+    <t>trussell copy.bib</t>
+  </si>
+  <si>
+    <t>trussellh.bib</t>
+  </si>
+  <si>
+    <t>turykn.bib</t>
+  </si>
+  <si>
+    <t>tyler copy.bib</t>
+  </si>
+  <si>
+    <t>urbenb.bib</t>
+  </si>
+  <si>
+    <t>vanbiersalt.bib</t>
+  </si>
+  <si>
+    <t>vandenbrookj.bib</t>
+  </si>
+  <si>
+    <t>vanryswykw.bib</t>
+  </si>
+  <si>
+    <t>victort.bib</t>
+  </si>
+  <si>
+    <t>wedbergj.bib</t>
+  </si>
+  <si>
+    <t>weissbacha.bib</t>
+  </si>
+  <si>
+    <t>wiersmaj.bib</t>
+  </si>
+  <si>
+    <t>wiestersenr.bib</t>
+  </si>
+  <si>
+    <t>wilsonb.bib</t>
+  </si>
+  <si>
+    <t>witthopfj.bib</t>
+  </si>
+  <si>
+    <t>wolfs.bib</t>
+  </si>
+  <si>
+    <t>zaporozeca.bib</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/adamst.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/albertsonp.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/alhajjarb.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/amesonp.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/andersonm.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/anklamj.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/armstrongd.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/attigj.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/ayres.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/baileyf.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/battistaj.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/Beaumiers.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/beckerg.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/belluckd.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/bentleyc.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/berndtj.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/berthouexp.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/blanchardm.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/blondeg.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/bohlingg.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/bohnm.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/bosscherp.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/bowenb.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/boyle copy.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/bradbury copy.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/brasino copy.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/breyk.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/brownb.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/browneb.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/bubenzerg.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/bundyl.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/catesk.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/chambersl.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/changm.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/chenc.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/cherkauer copy.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/chestersg.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/collinsm.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/connersk.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/converse copy.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/cowells.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/cruciani copy.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/curwend.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/danielt.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/davenportd.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/davidsond.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/delucad.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/detroitd.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/dobbinsb.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/doranf.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/doyled.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/dunnj.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/eatont.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/eldanm.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/evansw.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/eykholtg.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/falkp.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/fathullar.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/faublep.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/feinsteind.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/fermanichk.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/fishers.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/fitzgeraldc.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/friedmanm.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/fripiatj.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/geiss.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/gilbertt.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/goodmani.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/greent.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/greerb.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/grundlt.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/hamr.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/hansond.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/harkinj.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/harrism.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/harrisr.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/hartleyh.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/hartleyj.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/harveyr.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/heitmanm.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/helmkep.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/holmand.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/hoopes copy.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/hungerc.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/hutchinsonk.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/jelinskid.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/kammeld.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/kammererp.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/kanarekm.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/karasovw.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/kendye.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/kentera.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/knaakm.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/kopecky.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/kraftg.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/krohnc.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/kruele.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/lanl.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/lantzw.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/lawrencej.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/lemastersg.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/levyj.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/mccallisterr.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/mcgrathr.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/mckereghanp.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/mckinleyw.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/mechenichd.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/meisnerl.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/melbyj.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/mickelsond.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/monkmeyerp.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/mudreym.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/muhannaa.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/muldoon copy.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/murskyg.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/newenhousea.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/nienkeg.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/niewoehnerj.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/noelm.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/nollr.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/norenbergc.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/nowakp.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/omanb.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/osbornet.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/ostergrenc.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/otisr.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/palmerc.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/parkj.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/parsonsl.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/patochj.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/pauld.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/pawloskia.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/peerenboomd.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/pelczarj.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/peterson copy.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/porterw.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/portlet.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/posnerj.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/postlej.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/potterk.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/pughl.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/readh.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/richardsonn.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/roloffb.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/saltesj.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/sandstroml.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/sauerd.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/schalchl.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/schwalbej.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/seyboldc.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/shrawder.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/simot.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/simsimang.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/singhp.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/slanek.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/smallg.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/sonzogni copy.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/sorensonj.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/stieglitzr.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/stollr.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/strandridgej.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/suchtm.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/svavarssong.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/taylorr.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/tinkerj.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/trappp.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/travism.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/trussellh.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/turykn.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/tyler copy.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/urbenb.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/vanbiersalt.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/vandenbrookj.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/vanryswykw.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/victort.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/wedbergj.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/weissbacha.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/wiersmaj.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/wiestersenr.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/wilsonb.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/witthopfj.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/wolfs.bib", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"/Users/Amber/Documents/GitHub/GW_IA/authorsgs/zaporozeca.bib", </t>
   </si>
 </sst>
 </file>
@@ -1258,8 +2326,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1277,19 +2353,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1619,21 +2703,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J98"/>
+  <dimension ref="A1:J286"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H98"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H266"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="2" max="2" width="5.33203125" customWidth="1"/>
+    <col min="3" max="3" width="4.1640625" customWidth="1"/>
+    <col min="5" max="5" width="4" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
     <col min="8" max="8" width="60.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.6640625" customWidth="1"/>
+    <col min="9" max="9" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>382</v>
       </c>
       <c r="B1" t="s">
         <v>98</v>
@@ -1651,7 +2739,7 @@
         <v>298</v>
       </c>
       <c r="H1" t="s">
-        <v>299</v>
+        <v>570</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>100</v>
@@ -1659,7 +2747,7 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>383</v>
       </c>
       <c r="D2" t="s">
         <v>102</v>
@@ -1668,7 +2756,7 @@
         <v>201</v>
       </c>
       <c r="H2" t="s">
-        <v>300</v>
+        <v>571</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>199</v>
@@ -1676,7 +2764,7 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>384</v>
       </c>
       <c r="D3" t="s">
         <v>103</v>
@@ -1685,12 +2773,12 @@
         <v>202</v>
       </c>
       <c r="H3" t="s">
-        <v>301</v>
+        <v>572</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>385</v>
       </c>
       <c r="D4" t="s">
         <v>104</v>
@@ -1699,12 +2787,12 @@
         <v>203</v>
       </c>
       <c r="H4" t="s">
-        <v>302</v>
+        <v>573</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>386</v>
       </c>
       <c r="D5" t="s">
         <v>105</v>
@@ -1713,12 +2801,12 @@
         <v>204</v>
       </c>
       <c r="H5" t="s">
-        <v>303</v>
+        <v>574</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>387</v>
       </c>
       <c r="D6" t="s">
         <v>106</v>
@@ -1727,12 +2815,12 @@
         <v>205</v>
       </c>
       <c r="H6" t="s">
-        <v>304</v>
+        <v>575</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>388</v>
       </c>
       <c r="D7" t="s">
         <v>107</v>
@@ -1741,12 +2829,12 @@
         <v>206</v>
       </c>
       <c r="H7" t="s">
-        <v>305</v>
+        <v>576</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>389</v>
       </c>
       <c r="D8" t="s">
         <v>108</v>
@@ -1755,12 +2843,12 @@
         <v>207</v>
       </c>
       <c r="H8" t="s">
-        <v>306</v>
+        <v>577</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>390</v>
       </c>
       <c r="D9" t="s">
         <v>109</v>
@@ -1769,12 +2857,12 @@
         <v>208</v>
       </c>
       <c r="H9" t="s">
-        <v>307</v>
+        <v>578</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D10" t="s">
         <v>110</v>
@@ -1783,12 +2871,12 @@
         <v>209</v>
       </c>
       <c r="H10" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>391</v>
       </c>
       <c r="D11" t="s">
         <v>111</v>
@@ -1797,12 +2885,12 @@
         <v>210</v>
       </c>
       <c r="H11" t="s">
-        <v>309</v>
+        <v>579</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D12" t="s">
         <v>112</v>
@@ -1811,12 +2899,12 @@
         <v>211</v>
       </c>
       <c r="H12" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D13" t="s">
         <v>113</v>
@@ -1825,12 +2913,12 @@
         <v>212</v>
       </c>
       <c r="H13" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="D14" t="s">
         <v>114</v>
@@ -1839,12 +2927,12 @@
         <v>213</v>
       </c>
       <c r="H14" t="s">
-        <v>312</v>
+        <v>302</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>392</v>
       </c>
       <c r="D15" t="s">
         <v>115</v>
@@ -1853,12 +2941,12 @@
         <v>214</v>
       </c>
       <c r="H15" t="s">
-        <v>313</v>
+        <v>580</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>393</v>
       </c>
       <c r="D16" t="s">
         <v>116</v>
@@ -1867,12 +2955,12 @@
         <v>215</v>
       </c>
       <c r="H16" t="s">
-        <v>314</v>
+        <v>581</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>394</v>
       </c>
       <c r="D17" t="s">
         <v>117</v>
@@ -1881,12 +2969,12 @@
         <v>216</v>
       </c>
       <c r="H17" t="s">
-        <v>315</v>
+        <v>582</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>395</v>
       </c>
       <c r="D18" t="s">
         <v>118</v>
@@ -1895,12 +2983,12 @@
         <v>217</v>
       </c>
       <c r="H18" t="s">
-        <v>316</v>
+        <v>583</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>396</v>
       </c>
       <c r="D19" t="s">
         <v>119</v>
@@ -1909,12 +2997,12 @@
         <v>218</v>
       </c>
       <c r="H19" t="s">
-        <v>317</v>
+        <v>584</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>397</v>
       </c>
       <c r="D20" t="s">
         <v>120</v>
@@ -1923,12 +3011,12 @@
         <v>219</v>
       </c>
       <c r="H20" t="s">
-        <v>318</v>
+        <v>585</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>398</v>
       </c>
       <c r="D21" t="s">
         <v>121</v>
@@ -1937,12 +3025,12 @@
         <v>220</v>
       </c>
       <c r="H21" t="s">
-        <v>319</v>
+        <v>586</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>399</v>
       </c>
       <c r="D22" t="s">
         <v>122</v>
@@ -1951,12 +3039,12 @@
         <v>221</v>
       </c>
       <c r="H22" t="s">
-        <v>320</v>
+        <v>587</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>400</v>
       </c>
       <c r="D23" t="s">
         <v>123</v>
@@ -1965,12 +3053,12 @@
         <v>222</v>
       </c>
       <c r="H23" t="s">
-        <v>321</v>
+        <v>588</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>401</v>
       </c>
       <c r="D24" t="s">
         <v>124</v>
@@ -1979,12 +3067,12 @@
         <v>223</v>
       </c>
       <c r="H24" t="s">
-        <v>322</v>
+        <v>589</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>402</v>
       </c>
       <c r="D25" t="s">
         <v>125</v>
@@ -1993,12 +3081,12 @@
         <v>224</v>
       </c>
       <c r="H25" t="s">
-        <v>323</v>
+        <v>590</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>403</v>
       </c>
       <c r="D26" t="s">
         <v>126</v>
@@ -2007,12 +3095,12 @@
         <v>225</v>
       </c>
       <c r="H26" t="s">
-        <v>324</v>
+        <v>591</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>404</v>
       </c>
       <c r="D27" t="s">
         <v>127</v>
@@ -2021,12 +3109,12 @@
         <v>226</v>
       </c>
       <c r="H27" t="s">
-        <v>325</v>
+        <v>592</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="D28" t="s">
         <v>128</v>
@@ -2035,12 +3123,12 @@
         <v>227</v>
       </c>
       <c r="H28" t="s">
-        <v>326</v>
+        <v>303</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="D29" t="s">
         <v>129</v>
@@ -2049,12 +3137,12 @@
         <v>228</v>
       </c>
       <c r="H29" t="s">
-        <v>327</v>
+        <v>304</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>405</v>
       </c>
       <c r="D30" t="s">
         <v>130</v>
@@ -2063,12 +3151,12 @@
         <v>229</v>
       </c>
       <c r="H30" t="s">
-        <v>328</v>
+        <v>593</v>
       </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="D31" t="s">
         <v>131</v>
@@ -2077,12 +3165,12 @@
         <v>230</v>
       </c>
       <c r="H31" t="s">
-        <v>329</v>
+        <v>594</v>
       </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>406</v>
       </c>
       <c r="D32" t="s">
         <v>132</v>
@@ -2091,12 +3179,12 @@
         <v>231</v>
       </c>
       <c r="H32" t="s">
-        <v>330</v>
+        <v>595</v>
       </c>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="D33" t="s">
         <v>133</v>
@@ -2105,12 +3193,12 @@
         <v>232</v>
       </c>
       <c r="H33" t="s">
-        <v>331</v>
+        <v>305</v>
       </c>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>407</v>
       </c>
       <c r="D34" t="s">
         <v>134</v>
@@ -2119,12 +3207,12 @@
         <v>233</v>
       </c>
       <c r="H34" t="s">
-        <v>332</v>
+        <v>596</v>
       </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>408</v>
       </c>
       <c r="D35" t="s">
         <v>135</v>
@@ -2133,12 +3221,12 @@
         <v>234</v>
       </c>
       <c r="H35" t="s">
-        <v>333</v>
+        <v>597</v>
       </c>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="D36" t="s">
         <v>136</v>
@@ -2147,12 +3235,12 @@
         <v>235</v>
       </c>
       <c r="H36" t="s">
-        <v>334</v>
+        <v>598</v>
       </c>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="D37" t="s">
         <v>137</v>
@@ -2161,12 +3249,12 @@
         <v>236</v>
       </c>
       <c r="H37" t="s">
-        <v>335</v>
+        <v>306</v>
       </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>409</v>
       </c>
       <c r="D38" t="s">
         <v>138</v>
@@ -2175,12 +3263,12 @@
         <v>237</v>
       </c>
       <c r="H38" t="s">
-        <v>336</v>
+        <v>599</v>
       </c>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>410</v>
       </c>
       <c r="D39" t="s">
         <v>139</v>
@@ -2189,12 +3277,12 @@
         <v>238</v>
       </c>
       <c r="H39" t="s">
-        <v>337</v>
+        <v>600</v>
       </c>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" t="s">
-        <v>39</v>
+        <v>411</v>
       </c>
       <c r="D40" t="s">
         <v>140</v>
@@ -2203,12 +3291,12 @@
         <v>239</v>
       </c>
       <c r="H40" t="s">
-        <v>338</v>
+        <v>307</v>
       </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="D41" t="s">
         <v>141</v>
@@ -2217,12 +3305,12 @@
         <v>240</v>
       </c>
       <c r="H41" t="s">
-        <v>339</v>
+        <v>601</v>
       </c>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" t="s">
-        <v>41</v>
+        <v>412</v>
       </c>
       <c r="D42" t="s">
         <v>142</v>
@@ -2231,12 +3319,12 @@
         <v>241</v>
       </c>
       <c r="H42" t="s">
-        <v>340</v>
+        <v>602</v>
       </c>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" t="s">
-        <v>42</v>
+        <v>413</v>
       </c>
       <c r="D43" t="s">
         <v>143</v>
@@ -2245,12 +3333,12 @@
         <v>242</v>
       </c>
       <c r="H43" t="s">
-        <v>341</v>
+        <v>603</v>
       </c>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="D44" t="s">
         <v>144</v>
@@ -2259,12 +3347,12 @@
         <v>243</v>
       </c>
       <c r="H44" t="s">
-        <v>342</v>
+        <v>604</v>
       </c>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" t="s">
-        <v>44</v>
+        <v>414</v>
       </c>
       <c r="D45" t="s">
         <v>145</v>
@@ -2273,12 +3361,12 @@
         <v>244</v>
       </c>
       <c r="H45" t="s">
-        <v>343</v>
+        <v>605</v>
       </c>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" t="s">
-        <v>45</v>
+        <v>415</v>
       </c>
       <c r="D46" t="s">
         <v>146</v>
@@ -2287,12 +3375,12 @@
         <v>245</v>
       </c>
       <c r="H46" t="s">
-        <v>344</v>
+        <v>606</v>
       </c>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" t="s">
-        <v>46</v>
+        <v>416</v>
       </c>
       <c r="D47" t="s">
         <v>147</v>
@@ -2301,12 +3389,12 @@
         <v>246</v>
       </c>
       <c r="H47" t="s">
-        <v>345</v>
+        <v>308</v>
       </c>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" t="s">
-        <v>47</v>
+        <v>417</v>
       </c>
       <c r="D48" t="s">
         <v>148</v>
@@ -2315,12 +3403,12 @@
         <v>247</v>
       </c>
       <c r="H48" t="s">
-        <v>346</v>
+        <v>309</v>
       </c>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" t="s">
-        <v>48</v>
+        <v>418</v>
       </c>
       <c r="D49" t="s">
         <v>149</v>
@@ -2329,12 +3417,12 @@
         <v>248</v>
       </c>
       <c r="H49" t="s">
-        <v>347</v>
+        <v>607</v>
       </c>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="D50" t="s">
         <v>150</v>
@@ -2343,12 +3431,12 @@
         <v>249</v>
       </c>
       <c r="H50" t="s">
-        <v>348</v>
+        <v>608</v>
       </c>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" t="s">
-        <v>50</v>
+        <v>419</v>
       </c>
       <c r="D51" t="s">
         <v>151</v>
@@ -2357,12 +3445,12 @@
         <v>250</v>
       </c>
       <c r="H51" t="s">
-        <v>349</v>
+        <v>609</v>
       </c>
     </row>
     <row r="52" spans="1:8">
       <c r="A52" t="s">
-        <v>51</v>
+        <v>13</v>
       </c>
       <c r="D52" t="s">
         <v>152</v>
@@ -2371,12 +3459,12 @@
         <v>251</v>
       </c>
       <c r="H52" t="s">
-        <v>350</v>
+        <v>610</v>
       </c>
     </row>
     <row r="53" spans="1:8">
       <c r="A53" t="s">
-        <v>52</v>
+        <v>14</v>
       </c>
       <c r="D53" t="s">
         <v>153</v>
@@ -2385,12 +3473,12 @@
         <v>252</v>
       </c>
       <c r="H53" t="s">
-        <v>351</v>
+        <v>611</v>
       </c>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" t="s">
-        <v>53</v>
+        <v>420</v>
       </c>
       <c r="D54" t="s">
         <v>154</v>
@@ -2399,12 +3487,12 @@
         <v>253</v>
       </c>
       <c r="H54" t="s">
-        <v>352</v>
+        <v>612</v>
       </c>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" t="s">
-        <v>54</v>
+        <v>421</v>
       </c>
       <c r="D55" t="s">
         <v>155</v>
@@ -2413,12 +3501,12 @@
         <v>254</v>
       </c>
       <c r="H55" t="s">
-        <v>353</v>
+        <v>613</v>
       </c>
     </row>
     <row r="56" spans="1:8">
       <c r="A56" t="s">
-        <v>55</v>
+        <v>422</v>
       </c>
       <c r="D56" t="s">
         <v>156</v>
@@ -2427,12 +3515,12 @@
         <v>255</v>
       </c>
       <c r="H56" t="s">
-        <v>354</v>
+        <v>614</v>
       </c>
     </row>
     <row r="57" spans="1:8">
       <c r="A57" t="s">
-        <v>56</v>
+        <v>15</v>
       </c>
       <c r="D57" t="s">
         <v>157</v>
@@ -2441,12 +3529,12 @@
         <v>256</v>
       </c>
       <c r="H57" t="s">
-        <v>355</v>
+        <v>615</v>
       </c>
     </row>
     <row r="58" spans="1:8">
       <c r="A58" t="s">
-        <v>57</v>
+        <v>423</v>
       </c>
       <c r="D58" t="s">
         <v>158</v>
@@ -2455,12 +3543,12 @@
         <v>257</v>
       </c>
       <c r="H58" t="s">
-        <v>356</v>
+        <v>616</v>
       </c>
     </row>
     <row r="59" spans="1:8">
       <c r="A59" t="s">
-        <v>58</v>
+        <v>424</v>
       </c>
       <c r="D59" t="s">
         <v>159</v>
@@ -2469,12 +3557,12 @@
         <v>258</v>
       </c>
       <c r="H59" t="s">
-        <v>357</v>
+        <v>617</v>
       </c>
     </row>
     <row r="60" spans="1:8">
       <c r="A60" t="s">
-        <v>59</v>
+        <v>16</v>
       </c>
       <c r="D60" t="s">
         <v>160</v>
@@ -2483,12 +3571,12 @@
         <v>259</v>
       </c>
       <c r="H60" t="s">
-        <v>358</v>
+        <v>310</v>
       </c>
     </row>
     <row r="61" spans="1:8">
       <c r="A61" t="s">
-        <v>60</v>
+        <v>425</v>
       </c>
       <c r="D61" t="s">
         <v>161</v>
@@ -2497,12 +3585,12 @@
         <v>260</v>
       </c>
       <c r="H61" t="s">
-        <v>359</v>
+        <v>618</v>
       </c>
     </row>
     <row r="62" spans="1:8">
       <c r="A62" t="s">
-        <v>61</v>
+        <v>426</v>
       </c>
       <c r="D62" t="s">
         <v>162</v>
@@ -2511,12 +3599,12 @@
         <v>261</v>
       </c>
       <c r="H62" t="s">
-        <v>360</v>
+        <v>311</v>
       </c>
     </row>
     <row r="63" spans="1:8">
       <c r="A63" t="s">
-        <v>62</v>
+        <v>427</v>
       </c>
       <c r="D63" t="s">
         <v>163</v>
@@ -2525,12 +3613,12 @@
         <v>262</v>
       </c>
       <c r="H63" t="s">
-        <v>361</v>
+        <v>619</v>
       </c>
     </row>
     <row r="64" spans="1:8">
       <c r="A64" t="s">
-        <v>63</v>
+        <v>428</v>
       </c>
       <c r="D64" t="s">
         <v>164</v>
@@ -2539,12 +3627,12 @@
         <v>263</v>
       </c>
       <c r="H64" t="s">
-        <v>362</v>
+        <v>620</v>
       </c>
     </row>
     <row r="65" spans="1:8">
       <c r="A65" t="s">
-        <v>64</v>
+        <v>429</v>
       </c>
       <c r="D65" t="s">
         <v>165</v>
@@ -2553,12 +3641,12 @@
         <v>264</v>
       </c>
       <c r="H65" t="s">
-        <v>363</v>
+        <v>312</v>
       </c>
     </row>
     <row r="66" spans="1:8">
       <c r="A66" t="s">
-        <v>65</v>
+        <v>430</v>
       </c>
       <c r="D66" t="s">
         <v>166</v>
@@ -2567,12 +3655,12 @@
         <v>265</v>
       </c>
       <c r="H66" t="s">
-        <v>364</v>
+        <v>621</v>
       </c>
     </row>
     <row r="67" spans="1:8">
       <c r="A67" t="s">
-        <v>66</v>
+        <v>17</v>
       </c>
       <c r="D67" t="s">
         <v>167</v>
@@ -2581,12 +3669,12 @@
         <v>266</v>
       </c>
       <c r="H67" t="s">
-        <v>365</v>
+        <v>622</v>
       </c>
     </row>
     <row r="68" spans="1:8">
       <c r="A68" t="s">
-        <v>67</v>
+        <v>431</v>
       </c>
       <c r="D68" t="s">
         <v>168</v>
@@ -2595,12 +3683,12 @@
         <v>267</v>
       </c>
       <c r="H68" t="s">
-        <v>366</v>
+        <v>313</v>
       </c>
     </row>
     <row r="69" spans="1:8">
       <c r="A69" t="s">
-        <v>68</v>
+        <v>18</v>
       </c>
       <c r="D69" t="s">
         <v>169</v>
@@ -2609,12 +3697,12 @@
         <v>268</v>
       </c>
       <c r="H69" t="s">
-        <v>367</v>
+        <v>623</v>
       </c>
     </row>
     <row r="70" spans="1:8">
       <c r="A70" t="s">
-        <v>69</v>
+        <v>432</v>
       </c>
       <c r="D70" t="s">
         <v>170</v>
@@ -2623,12 +3711,12 @@
         <v>269</v>
       </c>
       <c r="H70" t="s">
-        <v>368</v>
+        <v>314</v>
       </c>
     </row>
     <row r="71" spans="1:8">
       <c r="A71" t="s">
-        <v>70</v>
+        <v>433</v>
       </c>
       <c r="D71" t="s">
         <v>171</v>
@@ -2637,12 +3725,12 @@
         <v>270</v>
       </c>
       <c r="H71" t="s">
-        <v>369</v>
+        <v>315</v>
       </c>
     </row>
     <row r="72" spans="1:8">
       <c r="A72" t="s">
-        <v>71</v>
+        <v>19</v>
       </c>
       <c r="D72" t="s">
         <v>172</v>
@@ -2651,12 +3739,12 @@
         <v>271</v>
       </c>
       <c r="H72" t="s">
-        <v>370</v>
+        <v>624</v>
       </c>
     </row>
     <row r="73" spans="1:8">
       <c r="A73" t="s">
-        <v>72</v>
+        <v>434</v>
       </c>
       <c r="D73" t="s">
         <v>173</v>
@@ -2665,12 +3753,12 @@
         <v>272</v>
       </c>
       <c r="H73" t="s">
-        <v>371</v>
+        <v>625</v>
       </c>
     </row>
     <row r="74" spans="1:8">
       <c r="A74" t="s">
-        <v>73</v>
+        <v>435</v>
       </c>
       <c r="D74" t="s">
         <v>174</v>
@@ -2679,12 +3767,12 @@
         <v>273</v>
       </c>
       <c r="H74" t="s">
-        <v>372</v>
+        <v>626</v>
       </c>
     </row>
     <row r="75" spans="1:8">
       <c r="A75" t="s">
-        <v>74</v>
+        <v>20</v>
       </c>
       <c r="D75" t="s">
         <v>175</v>
@@ -2693,12 +3781,12 @@
         <v>274</v>
       </c>
       <c r="H75" t="s">
-        <v>373</v>
+        <v>627</v>
       </c>
     </row>
     <row r="76" spans="1:8">
       <c r="A76" t="s">
-        <v>75</v>
+        <v>436</v>
       </c>
       <c r="D76" t="s">
         <v>176</v>
@@ -2707,12 +3795,12 @@
         <v>275</v>
       </c>
       <c r="H76" t="s">
-        <v>374</v>
+        <v>628</v>
       </c>
     </row>
     <row r="77" spans="1:8">
       <c r="A77" t="s">
-        <v>76</v>
+        <v>21</v>
       </c>
       <c r="D77" t="s">
         <v>177</v>
@@ -2721,12 +3809,12 @@
         <v>276</v>
       </c>
       <c r="H77" t="s">
-        <v>375</v>
+        <v>629</v>
       </c>
     </row>
     <row r="78" spans="1:8">
       <c r="A78" t="s">
-        <v>77</v>
+        <v>22</v>
       </c>
       <c r="D78" t="s">
         <v>178</v>
@@ -2735,12 +3823,12 @@
         <v>277</v>
       </c>
       <c r="H78" t="s">
-        <v>376</v>
+        <v>630</v>
       </c>
     </row>
     <row r="79" spans="1:8">
       <c r="A79" t="s">
-        <v>78</v>
+        <v>437</v>
       </c>
       <c r="D79" t="s">
         <v>179</v>
@@ -2749,12 +3837,12 @@
         <v>278</v>
       </c>
       <c r="H79" t="s">
-        <v>377</v>
+        <v>631</v>
       </c>
     </row>
     <row r="80" spans="1:8">
       <c r="A80" t="s">
-        <v>79</v>
+        <v>438</v>
       </c>
       <c r="D80" t="s">
         <v>180</v>
@@ -2763,12 +3851,12 @@
         <v>279</v>
       </c>
       <c r="H80" t="s">
-        <v>378</v>
+        <v>632</v>
       </c>
     </row>
     <row r="81" spans="1:8">
       <c r="A81" t="s">
-        <v>80</v>
+        <v>439</v>
       </c>
       <c r="D81" t="s">
         <v>181</v>
@@ -2777,12 +3865,12 @@
         <v>280</v>
       </c>
       <c r="H81" t="s">
-        <v>379</v>
+        <v>633</v>
       </c>
     </row>
     <row r="82" spans="1:8">
       <c r="A82" t="s">
-        <v>81</v>
+        <v>440</v>
       </c>
       <c r="D82" t="s">
         <v>182</v>
@@ -2791,12 +3879,12 @@
         <v>281</v>
       </c>
       <c r="H82" t="s">
-        <v>380</v>
+        <v>634</v>
       </c>
     </row>
     <row r="83" spans="1:8">
       <c r="A83" t="s">
-        <v>82</v>
+        <v>441</v>
       </c>
       <c r="D83" t="s">
         <v>183</v>
@@ -2805,12 +3893,12 @@
         <v>282</v>
       </c>
       <c r="H83" t="s">
-        <v>381</v>
+        <v>316</v>
       </c>
     </row>
     <row r="84" spans="1:8">
       <c r="A84" t="s">
-        <v>83</v>
+        <v>442</v>
       </c>
       <c r="D84" t="s">
         <v>184</v>
@@ -2819,12 +3907,12 @@
         <v>283</v>
       </c>
       <c r="H84" t="s">
-        <v>382</v>
+        <v>635</v>
       </c>
     </row>
     <row r="85" spans="1:8">
       <c r="A85" t="s">
-        <v>84</v>
+        <v>443</v>
       </c>
       <c r="D85" t="s">
         <v>185</v>
@@ -2833,12 +3921,12 @@
         <v>284</v>
       </c>
       <c r="H85" t="s">
-        <v>383</v>
+        <v>317</v>
       </c>
     </row>
     <row r="86" spans="1:8">
       <c r="A86" t="s">
-        <v>85</v>
+        <v>444</v>
       </c>
       <c r="D86" t="s">
         <v>186</v>
@@ -2847,12 +3935,12 @@
         <v>285</v>
       </c>
       <c r="H86" t="s">
-        <v>384</v>
+        <v>636</v>
       </c>
     </row>
     <row r="87" spans="1:8">
       <c r="A87" t="s">
-        <v>86</v>
+        <v>445</v>
       </c>
       <c r="D87" t="s">
         <v>187</v>
@@ -2861,12 +3949,12 @@
         <v>286</v>
       </c>
       <c r="H87" t="s">
-        <v>385</v>
+        <v>318</v>
       </c>
     </row>
     <row r="88" spans="1:8">
       <c r="A88" t="s">
-        <v>87</v>
+        <v>446</v>
       </c>
       <c r="D88" t="s">
         <v>188</v>
@@ -2875,12 +3963,12 @@
         <v>287</v>
       </c>
       <c r="H88" t="s">
-        <v>386</v>
+        <v>637</v>
       </c>
     </row>
     <row r="89" spans="1:8">
       <c r="A89" t="s">
-        <v>88</v>
+        <v>447</v>
       </c>
       <c r="D89" t="s">
         <v>189</v>
@@ -2889,12 +3977,12 @@
         <v>288</v>
       </c>
       <c r="H89" t="s">
-        <v>387</v>
+        <v>319</v>
       </c>
     </row>
     <row r="90" spans="1:8">
       <c r="A90" t="s">
-        <v>89</v>
+        <v>23</v>
       </c>
       <c r="D90" t="s">
         <v>190</v>
@@ -2903,12 +3991,12 @@
         <v>289</v>
       </c>
       <c r="H90" t="s">
-        <v>388</v>
+        <v>638</v>
       </c>
     </row>
     <row r="91" spans="1:8">
       <c r="A91" t="s">
-        <v>90</v>
+        <v>448</v>
       </c>
       <c r="D91" t="s">
         <v>191</v>
@@ -2917,12 +4005,12 @@
         <v>290</v>
       </c>
       <c r="H91" t="s">
-        <v>389</v>
+        <v>639</v>
       </c>
     </row>
     <row r="92" spans="1:8">
       <c r="A92" t="s">
-        <v>91</v>
+        <v>24</v>
       </c>
       <c r="D92" t="s">
         <v>192</v>
@@ -2931,12 +4019,12 @@
         <v>291</v>
       </c>
       <c r="H92" t="s">
-        <v>390</v>
+        <v>320</v>
       </c>
     </row>
     <row r="93" spans="1:8">
       <c r="A93" t="s">
-        <v>92</v>
+        <v>449</v>
       </c>
       <c r="D93" t="s">
         <v>193</v>
@@ -2945,12 +4033,12 @@
         <v>292</v>
       </c>
       <c r="H93" t="s">
-        <v>391</v>
+        <v>640</v>
       </c>
     </row>
     <row r="94" spans="1:8">
       <c r="A94" t="s">
-        <v>93</v>
+        <v>25</v>
       </c>
       <c r="D94" t="s">
         <v>194</v>
@@ -2959,12 +4047,12 @@
         <v>293</v>
       </c>
       <c r="H94" t="s">
-        <v>392</v>
+        <v>321</v>
       </c>
     </row>
     <row r="95" spans="1:8">
       <c r="A95" t="s">
-        <v>94</v>
+        <v>450</v>
       </c>
       <c r="D95" t="s">
         <v>195</v>
@@ -2973,12 +4061,12 @@
         <v>294</v>
       </c>
       <c r="H95" t="s">
-        <v>393</v>
+        <v>641</v>
       </c>
     </row>
     <row r="96" spans="1:8">
       <c r="A96" t="s">
-        <v>95</v>
+        <v>26</v>
       </c>
       <c r="D96" t="s">
         <v>196</v>
@@ -2987,12 +4075,12 @@
         <v>295</v>
       </c>
       <c r="H96" t="s">
-        <v>394</v>
+        <v>642</v>
       </c>
     </row>
     <row r="97" spans="1:8">
       <c r="A97" t="s">
-        <v>96</v>
+        <v>451</v>
       </c>
       <c r="D97" t="s">
         <v>197</v>
@@ -3001,12 +4089,12 @@
         <v>296</v>
       </c>
       <c r="H97" t="s">
-        <v>395</v>
+        <v>643</v>
       </c>
     </row>
     <row r="98" spans="1:8">
       <c r="A98" t="s">
-        <v>97</v>
+        <v>452</v>
       </c>
       <c r="D98" t="s">
         <v>198</v>
@@ -3015,10 +4103,1457 @@
         <v>297</v>
       </c>
       <c r="H98" t="s">
-        <v>396</v>
+        <v>644</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8">
+      <c r="A99" t="s">
+        <v>27</v>
+      </c>
+      <c r="H99" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8">
+      <c r="A100" t="s">
+        <v>453</v>
+      </c>
+      <c r="H100" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8">
+      <c r="A101" t="s">
+        <v>28</v>
+      </c>
+      <c r="H101" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8">
+      <c r="A102" t="s">
+        <v>454</v>
+      </c>
+      <c r="H102" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8">
+      <c r="A103" t="s">
+        <v>455</v>
+      </c>
+      <c r="H103" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8">
+      <c r="A104" t="s">
+        <v>456</v>
+      </c>
+      <c r="H104" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8">
+      <c r="A105" t="s">
+        <v>457</v>
+      </c>
+      <c r="H105" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8">
+      <c r="A106" t="s">
+        <v>458</v>
+      </c>
+      <c r="H106" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8">
+      <c r="A107" t="s">
+        <v>459</v>
+      </c>
+      <c r="H107" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8">
+      <c r="A108" t="s">
+        <v>460</v>
+      </c>
+      <c r="H108" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8">
+      <c r="A109" t="s">
+        <v>461</v>
+      </c>
+      <c r="H109" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8">
+      <c r="A110" t="s">
+        <v>29</v>
+      </c>
+      <c r="H110" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8">
+      <c r="A111" t="s">
+        <v>462</v>
+      </c>
+      <c r="H111" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8">
+      <c r="A112" t="s">
+        <v>463</v>
+      </c>
+      <c r="H112" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8">
+      <c r="A113" t="s">
+        <v>30</v>
+      </c>
+      <c r="H113" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8">
+      <c r="A114" t="s">
+        <v>464</v>
+      </c>
+      <c r="H114" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8">
+      <c r="A115" t="s">
+        <v>465</v>
+      </c>
+      <c r="H115" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8">
+      <c r="A116" t="s">
+        <v>31</v>
+      </c>
+      <c r="H116" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8">
+      <c r="A117" t="s">
+        <v>32</v>
+      </c>
+      <c r="H117" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8">
+      <c r="A118" t="s">
+        <v>466</v>
+      </c>
+      <c r="H118" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8">
+      <c r="A119" t="s">
+        <v>33</v>
+      </c>
+      <c r="H119" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8">
+      <c r="A120" t="s">
+        <v>467</v>
+      </c>
+      <c r="H120" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8">
+      <c r="A121" t="s">
+        <v>468</v>
+      </c>
+      <c r="H121" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8">
+      <c r="A122" t="s">
+        <v>34</v>
+      </c>
+      <c r="H122" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8">
+      <c r="A123" t="s">
+        <v>469</v>
+      </c>
+      <c r="H123" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8">
+      <c r="A124" t="s">
+        <v>470</v>
+      </c>
+      <c r="H124" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8">
+      <c r="A125" t="s">
+        <v>471</v>
+      </c>
+      <c r="H125" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8">
+      <c r="A126" t="s">
+        <v>472</v>
+      </c>
+      <c r="H126" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8">
+      <c r="A127" t="s">
+        <v>35</v>
+      </c>
+      <c r="H127" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8">
+      <c r="A128" t="s">
+        <v>473</v>
+      </c>
+      <c r="H128" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8">
+      <c r="A129" t="s">
+        <v>474</v>
+      </c>
+      <c r="H129" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8">
+      <c r="A130" t="s">
+        <v>36</v>
+      </c>
+      <c r="H130" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8">
+      <c r="A131" t="s">
+        <v>37</v>
+      </c>
+      <c r="H131" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8">
+      <c r="A132" t="s">
+        <v>475</v>
+      </c>
+      <c r="H132" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8">
+      <c r="A133" t="s">
+        <v>38</v>
+      </c>
+      <c r="H133" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8">
+      <c r="A134" t="s">
+        <v>476</v>
+      </c>
+      <c r="H134" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8">
+      <c r="A135" t="s">
+        <v>477</v>
+      </c>
+      <c r="H135" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8">
+      <c r="A136" t="s">
+        <v>39</v>
+      </c>
+      <c r="H136" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8">
+      <c r="A137" t="s">
+        <v>478</v>
+      </c>
+      <c r="H137" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8">
+      <c r="A138" t="s">
+        <v>479</v>
+      </c>
+      <c r="H138" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8">
+      <c r="A139" t="s">
+        <v>480</v>
+      </c>
+      <c r="H139" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8">
+      <c r="A140" t="s">
+        <v>40</v>
+      </c>
+      <c r="H140" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8">
+      <c r="A141" t="s">
+        <v>41</v>
+      </c>
+      <c r="H141" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8">
+      <c r="A142" t="s">
+        <v>42</v>
+      </c>
+      <c r="H142" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8">
+      <c r="A143" t="s">
+        <v>481</v>
+      </c>
+      <c r="H143" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8">
+      <c r="A144" t="s">
+        <v>482</v>
+      </c>
+      <c r="H144" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8">
+      <c r="A145" t="s">
+        <v>43</v>
+      </c>
+      <c r="H145" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8">
+      <c r="A146" t="s">
+        <v>44</v>
+      </c>
+      <c r="H146" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8">
+      <c r="A147" t="s">
+        <v>483</v>
+      </c>
+      <c r="H147" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8">
+      <c r="A148" t="s">
+        <v>484</v>
+      </c>
+      <c r="H148" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8">
+      <c r="A149" t="s">
+        <v>45</v>
+      </c>
+      <c r="H149" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8">
+      <c r="A150" t="s">
+        <v>46</v>
+      </c>
+      <c r="H150" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8">
+      <c r="A151" t="s">
+        <v>485</v>
+      </c>
+      <c r="H151" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8">
+      <c r="A152" t="s">
+        <v>47</v>
+      </c>
+      <c r="H152" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8">
+      <c r="A153" t="s">
+        <v>48</v>
+      </c>
+      <c r="H153" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8">
+      <c r="A154" t="s">
+        <v>49</v>
+      </c>
+      <c r="H154" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8">
+      <c r="A155" t="s">
+        <v>50</v>
+      </c>
+      <c r="H155" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8">
+      <c r="A156" t="s">
+        <v>51</v>
+      </c>
+      <c r="H156" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8">
+      <c r="A157" t="s">
+        <v>52</v>
+      </c>
+      <c r="H157" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8">
+      <c r="A158" t="s">
+        <v>53</v>
+      </c>
+      <c r="H158" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8">
+      <c r="A159" t="s">
+        <v>54</v>
+      </c>
+      <c r="H159" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8">
+      <c r="A160" t="s">
+        <v>55</v>
+      </c>
+      <c r="H160" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8">
+      <c r="A161" t="s">
+        <v>486</v>
+      </c>
+      <c r="H161" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8">
+      <c r="A162" t="s">
+        <v>56</v>
+      </c>
+      <c r="H162" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8">
+      <c r="A163" t="s">
+        <v>57</v>
+      </c>
+      <c r="H163" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8">
+      <c r="A164" t="s">
+        <v>487</v>
+      </c>
+      <c r="H164" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8">
+      <c r="A165" t="s">
+        <v>58</v>
+      </c>
+      <c r="H165" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8">
+      <c r="A166" t="s">
+        <v>59</v>
+      </c>
+      <c r="H166" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8">
+      <c r="A167" t="s">
+        <v>488</v>
+      </c>
+      <c r="H167" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8">
+      <c r="A168" t="s">
+        <v>489</v>
+      </c>
+      <c r="H168" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8">
+      <c r="A169" t="s">
+        <v>60</v>
+      </c>
+      <c r="H169" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8">
+      <c r="A170" t="s">
+        <v>490</v>
+      </c>
+      <c r="H170" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8">
+      <c r="A171" t="s">
+        <v>491</v>
+      </c>
+      <c r="H171" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8">
+      <c r="A172" t="s">
+        <v>492</v>
+      </c>
+      <c r="H172" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8">
+      <c r="A173" t="s">
+        <v>493</v>
+      </c>
+      <c r="H173" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8">
+      <c r="A174" t="s">
+        <v>494</v>
+      </c>
+      <c r="H174" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8">
+      <c r="A175" t="s">
+        <v>495</v>
+      </c>
+      <c r="H175" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="176" spans="1:8">
+      <c r="A176" t="s">
+        <v>496</v>
+      </c>
+      <c r="H176" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="177" spans="1:8">
+      <c r="A177" t="s">
+        <v>497</v>
+      </c>
+      <c r="H177" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="178" spans="1:8">
+      <c r="A178" t="s">
+        <v>61</v>
+      </c>
+      <c r="H178" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8">
+      <c r="A179" t="s">
+        <v>498</v>
+      </c>
+      <c r="H179" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="180" spans="1:8">
+      <c r="A180" t="s">
+        <v>499</v>
+      </c>
+      <c r="H180" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="181" spans="1:8">
+      <c r="A181" t="s">
+        <v>500</v>
+      </c>
+      <c r="H181" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="182" spans="1:8">
+      <c r="A182" t="s">
+        <v>501</v>
+      </c>
+      <c r="H182" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="183" spans="1:8">
+      <c r="A183" t="s">
+        <v>62</v>
+      </c>
+      <c r="H183" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="184" spans="1:8">
+      <c r="A184" t="s">
+        <v>502</v>
+      </c>
+      <c r="H184" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="185" spans="1:8">
+      <c r="A185" t="s">
+        <v>503</v>
+      </c>
+      <c r="H185" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="186" spans="1:8">
+      <c r="A186" t="s">
+        <v>504</v>
+      </c>
+      <c r="H186" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="187" spans="1:8">
+      <c r="A187" t="s">
+        <v>63</v>
+      </c>
+      <c r="H187" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="188" spans="1:8">
+      <c r="A188" t="s">
+        <v>505</v>
+      </c>
+      <c r="H188" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="189" spans="1:8">
+      <c r="A189" t="s">
+        <v>64</v>
+      </c>
+      <c r="H189" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="190" spans="1:8">
+      <c r="A190" t="s">
+        <v>65</v>
+      </c>
+      <c r="H190" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="191" spans="1:8">
+      <c r="A191" t="s">
+        <v>506</v>
+      </c>
+      <c r="H191" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="192" spans="1:8">
+      <c r="A192" t="s">
+        <v>507</v>
+      </c>
+      <c r="H192" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="193" spans="1:8">
+      <c r="A193" t="s">
+        <v>508</v>
+      </c>
+      <c r="H193" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="194" spans="1:8">
+      <c r="A194" t="s">
+        <v>509</v>
+      </c>
+      <c r="H194" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="195" spans="1:8">
+      <c r="A195" t="s">
+        <v>66</v>
+      </c>
+      <c r="H195" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="196" spans="1:8">
+      <c r="A196" t="s">
+        <v>510</v>
+      </c>
+      <c r="H196" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="197" spans="1:8">
+      <c r="A197" t="s">
+        <v>67</v>
+      </c>
+      <c r="H197" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="198" spans="1:8">
+      <c r="A198" t="s">
+        <v>511</v>
+      </c>
+      <c r="H198" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="199" spans="1:8">
+      <c r="A199" t="s">
+        <v>68</v>
+      </c>
+      <c r="H199" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="200" spans="1:8">
+      <c r="A200" t="s">
+        <v>512</v>
+      </c>
+      <c r="H200" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="201" spans="1:8">
+      <c r="A201" t="s">
+        <v>513</v>
+      </c>
+      <c r="H201" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="202" spans="1:8">
+      <c r="A202" t="s">
+        <v>514</v>
+      </c>
+      <c r="H202" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="203" spans="1:8">
+      <c r="A203" t="s">
+        <v>515</v>
+      </c>
+      <c r="H203" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="204" spans="1:8">
+      <c r="A204" t="s">
+        <v>69</v>
+      </c>
+      <c r="H204" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="205" spans="1:8">
+      <c r="A205" t="s">
+        <v>516</v>
+      </c>
+      <c r="H205" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="206" spans="1:8">
+      <c r="A206" t="s">
+        <v>517</v>
+      </c>
+      <c r="H206" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="207" spans="1:8">
+      <c r="A207" t="s">
+        <v>518</v>
+      </c>
+      <c r="H207" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="208" spans="1:8">
+      <c r="A208" t="s">
+        <v>70</v>
+      </c>
+      <c r="H208" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="209" spans="1:8">
+      <c r="A209" t="s">
+        <v>519</v>
+      </c>
+      <c r="H209" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="210" spans="1:8">
+      <c r="A210" t="s">
+        <v>520</v>
+      </c>
+      <c r="H210" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="211" spans="1:8">
+      <c r="A211" t="s">
+        <v>521</v>
+      </c>
+      <c r="H211" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="212" spans="1:8">
+      <c r="A212" t="s">
+        <v>522</v>
+      </c>
+      <c r="H212" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="213" spans="1:8">
+      <c r="A213" t="s">
+        <v>71</v>
+      </c>
+      <c r="H213" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="214" spans="1:8">
+      <c r="A214" t="s">
+        <v>523</v>
+      </c>
+      <c r="H214" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="215" spans="1:8">
+      <c r="A215" t="s">
+        <v>524</v>
+      </c>
+      <c r="H215" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="216" spans="1:8">
+      <c r="A216" t="s">
+        <v>525</v>
+      </c>
+      <c r="H216" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="217" spans="1:8">
+      <c r="A217" t="s">
+        <v>72</v>
+      </c>
+      <c r="H217" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="218" spans="1:8">
+      <c r="A218" t="s">
+        <v>526</v>
+      </c>
+      <c r="H218" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="219" spans="1:8">
+      <c r="A219" t="s">
+        <v>73</v>
+      </c>
+      <c r="H219" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="220" spans="1:8">
+      <c r="A220" t="s">
+        <v>527</v>
+      </c>
+      <c r="H220" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="221" spans="1:8">
+      <c r="A221" t="s">
+        <v>528</v>
+      </c>
+      <c r="H221" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="222" spans="1:8">
+      <c r="A222" t="s">
+        <v>74</v>
+      </c>
+      <c r="H222" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="223" spans="1:8">
+      <c r="A223" t="s">
+        <v>75</v>
+      </c>
+      <c r="H223" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="224" spans="1:8">
+      <c r="A224" t="s">
+        <v>529</v>
+      </c>
+      <c r="H224" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="225" spans="1:8">
+      <c r="A225" t="s">
+        <v>530</v>
+      </c>
+      <c r="H225" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="226" spans="1:8">
+      <c r="A226" t="s">
+        <v>531</v>
+      </c>
+      <c r="H226" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="227" spans="1:8">
+      <c r="A227" t="s">
+        <v>532</v>
+      </c>
+      <c r="H227" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="228" spans="1:8">
+      <c r="A228" t="s">
+        <v>76</v>
+      </c>
+      <c r="H228" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="229" spans="1:8">
+      <c r="A229" t="s">
+        <v>77</v>
+      </c>
+      <c r="H229" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="230" spans="1:8">
+      <c r="A230" t="s">
+        <v>533</v>
+      </c>
+      <c r="H230" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="231" spans="1:8">
+      <c r="A231" t="s">
+        <v>78</v>
+      </c>
+      <c r="H231" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="232" spans="1:8">
+      <c r="A232" t="s">
+        <v>534</v>
+      </c>
+      <c r="H232" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="233" spans="1:8">
+      <c r="A233" t="s">
+        <v>79</v>
+      </c>
+      <c r="H233" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="234" spans="1:8">
+      <c r="A234" t="s">
+        <v>80</v>
+      </c>
+      <c r="H234" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="235" spans="1:8">
+      <c r="A235" t="s">
+        <v>535</v>
+      </c>
+      <c r="H235" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="236" spans="1:8">
+      <c r="A236" t="s">
+        <v>536</v>
+      </c>
+      <c r="H236" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="237" spans="1:8">
+      <c r="A237" t="s">
+        <v>537</v>
+      </c>
+      <c r="H237" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="238" spans="1:8">
+      <c r="A238" t="s">
+        <v>538</v>
+      </c>
+      <c r="H238" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="239" spans="1:8">
+      <c r="A239" t="s">
+        <v>81</v>
+      </c>
+      <c r="H239" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="240" spans="1:8">
+      <c r="A240" t="s">
+        <v>539</v>
+      </c>
+      <c r="H240" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="241" spans="1:8">
+      <c r="A241" t="s">
+        <v>540</v>
+      </c>
+      <c r="H241" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="242" spans="1:8">
+      <c r="A242" t="s">
+        <v>541</v>
+      </c>
+      <c r="H242" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="243" spans="1:8">
+      <c r="A243" t="s">
+        <v>82</v>
+      </c>
+      <c r="H243" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="244" spans="1:8">
+      <c r="A244" t="s">
+        <v>542</v>
+      </c>
+      <c r="H244" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="245" spans="1:8">
+      <c r="A245" t="s">
+        <v>83</v>
+      </c>
+      <c r="H245" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="246" spans="1:8">
+      <c r="A246" t="s">
+        <v>84</v>
+      </c>
+      <c r="H246" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="247" spans="1:8">
+      <c r="A247" t="s">
+        <v>85</v>
+      </c>
+      <c r="H247" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="248" spans="1:8">
+      <c r="A248" t="s">
+        <v>543</v>
+      </c>
+      <c r="H248" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="249" spans="1:8">
+      <c r="A249" t="s">
+        <v>544</v>
+      </c>
+      <c r="H249" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="250" spans="1:8">
+      <c r="A250" t="s">
+        <v>86</v>
+      </c>
+      <c r="H250" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="251" spans="1:8">
+      <c r="A251" t="s">
+        <v>545</v>
+      </c>
+      <c r="H251" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="252" spans="1:8">
+      <c r="A252" t="s">
+        <v>546</v>
+      </c>
+      <c r="H252" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="253" spans="1:8">
+      <c r="A253" t="s">
+        <v>87</v>
+      </c>
+      <c r="H253" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="254" spans="1:8">
+      <c r="A254" t="s">
+        <v>547</v>
+      </c>
+      <c r="H254" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="255" spans="1:8">
+      <c r="A255" t="s">
+        <v>548</v>
+      </c>
+      <c r="H255" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="256" spans="1:8">
+      <c r="A256" t="s">
+        <v>88</v>
+      </c>
+      <c r="H256" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="257" spans="1:8">
+      <c r="A257" t="s">
+        <v>89</v>
+      </c>
+      <c r="H257" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="258" spans="1:8">
+      <c r="A258" t="s">
+        <v>549</v>
+      </c>
+      <c r="H258" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="259" spans="1:8">
+      <c r="A259" t="s">
+        <v>550</v>
+      </c>
+      <c r="H259" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="260" spans="1:8">
+      <c r="A260" t="s">
+        <v>551</v>
+      </c>
+      <c r="H260" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="261" spans="1:8">
+      <c r="A261" t="s">
+        <v>552</v>
+      </c>
+      <c r="H261" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="262" spans="1:8">
+      <c r="A262" t="s">
+        <v>553</v>
+      </c>
+      <c r="H262" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="263" spans="1:8">
+      <c r="A263" t="s">
+        <v>90</v>
+      </c>
+      <c r="H263" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="264" spans="1:8">
+      <c r="A264" t="s">
+        <v>554</v>
+      </c>
+      <c r="H264" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="265" spans="1:8">
+      <c r="A265" t="s">
+        <v>555</v>
+      </c>
+      <c r="H265" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="266" spans="1:8">
+      <c r="A266" t="s">
+        <v>556</v>
+      </c>
+      <c r="H266" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="267" spans="1:8">
+      <c r="A267" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="268" spans="1:8">
+      <c r="A268" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="269" spans="1:8">
+      <c r="A269" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="270" spans="1:8">
+      <c r="A270" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="271" spans="1:8">
+      <c r="A271" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="272" spans="1:8">
+      <c r="A272" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="273" spans="1:1">
+      <c r="A273" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="274" spans="1:1">
+      <c r="A274" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="275" spans="1:1">
+      <c r="A275" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="276" spans="1:1">
+      <c r="A276" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="277" spans="1:1">
+      <c r="A277" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="278" spans="1:1">
+      <c r="A278" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="279" spans="1:1">
+      <c r="A279" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="280" spans="1:1">
+      <c r="A280" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="281" spans="1:1">
+      <c r="A281" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="282" spans="1:1">
+      <c r="A282" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="283" spans="1:1">
+      <c r="A283" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="284" spans="1:1">
+      <c r="A284" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="285" spans="1:1">
+      <c r="A285" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="286" spans="1:1">
+      <c r="A286" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="H1:H286">
+    <sortCondition ref="H1"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>